<commit_message>
New Data September 5
New Data September 5
</commit_message>
<xml_diff>
--- a/covid19.xlsx
+++ b/covid19.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariah.birgen\Dropbox\2019-2020\Winter 2020\COVID19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BC5B87-5688-48AD-9A0D-FCD19028D804}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E914755E-A0BB-48BB-92C0-1CA7D10CE060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,13 +1091,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AS171"/>
+  <dimension ref="A1:AS173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X154" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AA154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI171" sqref="AI171"/>
+      <selection pane="bottomRight" activeCell="AL173" sqref="AL173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10700,11 +10700,11 @@
         <v>879</v>
       </c>
       <c r="R123">
-        <f t="shared" ref="R123" si="25">M123-M122</f>
+        <f t="shared" ref="R123:R154" si="25">M123-M122</f>
         <v>9221</v>
       </c>
       <c r="S123" s="8">
-        <f t="shared" ref="S123" si="26">Q123/U123</f>
+        <f t="shared" ref="S123:S154" si="26">Q123/U123</f>
         <v>8.7029702970297024E-2</v>
       </c>
       <c r="T123" s="8">
@@ -10755,15 +10755,15 @@
         <v>60</v>
       </c>
       <c r="AH123">
-        <f t="shared" ref="AH123" si="27">Y123-AB123-AE123</f>
+        <f t="shared" ref="AH123:AH154" si="27">Y123-AB123-AE123</f>
         <v>45</v>
       </c>
       <c r="AI123">
-        <f t="shared" ref="AI123" si="28">Z123-AC123-AF123</f>
+        <f t="shared" ref="AI123:AI154" si="28">Z123-AC123-AF123</f>
         <v>17</v>
       </c>
       <c r="AJ123">
-        <f t="shared" ref="AJ123" si="29">AA123-AD123-AG123</f>
+        <f t="shared" ref="AJ123:AJ154" si="29">AA123-AD123-AG123</f>
         <v>668</v>
       </c>
     </row>
@@ -10803,11 +10803,11 @@
         <v>287</v>
       </c>
       <c r="R124">
-        <f t="shared" ref="R124" si="30">M124-M123</f>
+        <f t="shared" si="25"/>
         <v>427</v>
       </c>
       <c r="S124" s="8">
-        <f t="shared" ref="S124" si="31">Q124/U124</f>
+        <f t="shared" si="26"/>
         <v>0.40196078431372551</v>
       </c>
       <c r="T124" s="8">
@@ -10858,15 +10858,15 @@
         <v>60</v>
       </c>
       <c r="AH124">
-        <f t="shared" ref="AH124" si="32">Y124-AB124-AE124</f>
+        <f t="shared" si="27"/>
         <v>45</v>
       </c>
       <c r="AI124">
-        <f t="shared" ref="AI124" si="33">Z124-AC124-AF124</f>
+        <f t="shared" si="28"/>
         <v>19</v>
       </c>
       <c r="AJ124">
-        <f t="shared" ref="AJ124" si="34">AA124-AD124-AG124</f>
+        <f t="shared" si="29"/>
         <v>669</v>
       </c>
     </row>
@@ -10906,11 +10906,11 @@
         <v>661</v>
       </c>
       <c r="R125">
-        <f t="shared" ref="R125" si="35">M125-M124</f>
+        <f t="shared" si="25"/>
         <v>10110</v>
       </c>
       <c r="S125" s="8">
-        <f t="shared" ref="S125" si="36">Q125/U125</f>
+        <f t="shared" si="26"/>
         <v>6.1368489462445455E-2</v>
       </c>
       <c r="T125" s="8">
@@ -10961,15 +10961,15 @@
         <v>60</v>
       </c>
       <c r="AH125">
-        <f t="shared" ref="AH125" si="37">Y125-AB125-AE125</f>
+        <f t="shared" si="27"/>
         <v>49</v>
       </c>
       <c r="AI125">
-        <f t="shared" ref="AI125" si="38">Z125-AC125-AF125</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ125">
-        <f t="shared" ref="AJ125" si="39">AA125-AD125-AG125</f>
+        <f t="shared" si="29"/>
         <v>693</v>
       </c>
     </row>
@@ -11009,15 +11009,15 @@
         <v>343</v>
       </c>
       <c r="R126">
-        <f t="shared" ref="R126" si="40">M126-M125</f>
+        <f t="shared" si="25"/>
         <v>4427</v>
       </c>
       <c r="S126" s="8">
-        <f t="shared" ref="S126" si="41">Q126/U126</f>
+        <f t="shared" si="26"/>
         <v>7.1907756813417184E-2</v>
       </c>
       <c r="T126" s="8">
-        <f t="shared" ref="T126:T133" si="42">SUM(Q120:Q126)/SUM(U120:U126)</f>
+        <f t="shared" ref="T126:T133" si="30">SUM(Q120:Q126)/SUM(U120:U126)</f>
         <v>8.1735039247221489E-2</v>
       </c>
       <c r="U126">
@@ -11064,15 +11064,15 @@
         <v>60</v>
       </c>
       <c r="AH126">
-        <f t="shared" ref="AH126" si="43">Y126-AB126-AE126</f>
+        <f t="shared" si="27"/>
         <v>49</v>
       </c>
       <c r="AI126">
-        <f t="shared" ref="AI126" si="44">Z126-AC126-AF126</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ126">
-        <f t="shared" ref="AJ126" si="45">AA126-AD126-AG126</f>
+        <f t="shared" si="29"/>
         <v>702</v>
       </c>
     </row>
@@ -11124,15 +11124,15 @@
         <v>512</v>
       </c>
       <c r="R127">
-        <f t="shared" ref="R127" si="46">M127-M126</f>
+        <f t="shared" si="25"/>
         <v>3442</v>
       </c>
       <c r="S127" s="8">
-        <f t="shared" ref="S127" si="47">Q127/U127</f>
+        <f t="shared" si="26"/>
         <v>0.12948912493677289</v>
       </c>
       <c r="T127" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>8.5611373503172564E-2</v>
       </c>
       <c r="U127">
@@ -11179,15 +11179,15 @@
         <v>60</v>
       </c>
       <c r="AH127">
-        <f t="shared" ref="AH127" si="48">Y127-AB127-AE127</f>
+        <f t="shared" si="27"/>
         <v>54</v>
       </c>
       <c r="AI127">
-        <f t="shared" ref="AI127" si="49">Z127-AC127-AF127</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ127">
-        <f t="shared" ref="AJ127" si="50">AA127-AD127-AG127</f>
+        <f t="shared" si="29"/>
         <v>713</v>
       </c>
     </row>
@@ -11239,15 +11239,15 @@
         <v>374</v>
       </c>
       <c r="R128">
-        <f t="shared" ref="R128" si="51">M128-M127</f>
+        <f t="shared" si="25"/>
         <v>4313</v>
       </c>
       <c r="S128" s="8">
-        <f t="shared" ref="S128" si="52">Q128/U128</f>
+        <f t="shared" si="26"/>
         <v>7.9795178152336249E-2</v>
       </c>
       <c r="T128" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>8.7082493104327474E-2</v>
       </c>
       <c r="U128">
@@ -11294,19 +11294,19 @@
         <v>61</v>
       </c>
       <c r="AH128">
-        <f t="shared" ref="AH128" si="53">Y128-AB128-AE128</f>
+        <f t="shared" si="27"/>
         <v>57</v>
       </c>
       <c r="AI128">
-        <f t="shared" ref="AI128" si="54">Z128-AC128-AF128</f>
+        <f t="shared" si="28"/>
         <v>18</v>
       </c>
       <c r="AJ128">
-        <f t="shared" ref="AJ128" si="55">AA128-AD128-AG128</f>
+        <f t="shared" si="29"/>
         <v>712</v>
       </c>
       <c r="AK128">
-        <f t="shared" ref="AK128:AK169" si="56">-(J128-J127)+L128</f>
+        <f t="shared" ref="AK128:AK169" si="31">-(J128-J127)+L128</f>
         <v>2</v>
       </c>
     </row>
@@ -11358,15 +11358,15 @@
         <v>716</v>
       </c>
       <c r="R129">
-        <f t="shared" ref="R129" si="57">M129-M128</f>
+        <f t="shared" si="25"/>
         <v>8110</v>
       </c>
       <c r="S129" s="8">
-        <f t="shared" ref="S129" si="58">Q129/U129</f>
+        <f t="shared" si="26"/>
         <v>8.1123951960117832E-2</v>
       </c>
       <c r="T129" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>8.607548719821094E-2</v>
       </c>
       <c r="U129">
@@ -11413,19 +11413,19 @@
         <v>61</v>
       </c>
       <c r="AH129">
-        <f t="shared" ref="AH129" si="59">Y129-AB129-AE129</f>
+        <f t="shared" si="27"/>
         <v>65</v>
       </c>
       <c r="AI129">
-        <f t="shared" ref="AI129" si="60">Z129-AC129-AF129</f>
+        <f t="shared" si="28"/>
         <v>19</v>
       </c>
       <c r="AJ129">
-        <f t="shared" ref="AJ129" si="61">AA129-AD129-AG129</f>
+        <f t="shared" si="29"/>
         <v>740</v>
       </c>
       <c r="AK129">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -11477,15 +11477,15 @@
         <v>451</v>
       </c>
       <c r="R130">
-        <f t="shared" ref="R130" si="62">M130-M129</f>
+        <f t="shared" si="25"/>
         <v>4071</v>
       </c>
       <c r="S130" s="8">
-        <f t="shared" ref="S130" si="63">Q130/U130</f>
+        <f t="shared" si="26"/>
         <v>9.9734630694383014E-2</v>
       </c>
       <c r="T130" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>8.7438552452672319E-2</v>
       </c>
       <c r="U130">
@@ -11532,19 +11532,19 @@
         <v>61</v>
       </c>
       <c r="AH130">
-        <f t="shared" ref="AH130" si="64">Y130-AB130-AE130</f>
+        <f t="shared" si="27"/>
         <v>68</v>
       </c>
       <c r="AI130">
-        <f t="shared" ref="AI130" si="65">Z130-AC130-AF130</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AJ130">
-        <f t="shared" ref="AJ130" si="66">AA130-AD130-AG130</f>
+        <f t="shared" si="29"/>
         <v>744</v>
       </c>
       <c r="AK130">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
     </row>
@@ -11596,15 +11596,15 @@
         <v>668</v>
       </c>
       <c r="R131">
-        <f t="shared" ref="R131" si="67">M131-M130</f>
+        <f t="shared" si="25"/>
         <v>5327</v>
       </c>
       <c r="S131" s="8">
-        <f t="shared" ref="S131" si="68">Q131/U131</f>
+        <f t="shared" si="26"/>
         <v>0.11142618849040867</v>
       </c>
       <c r="T131" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>8.5582998276852382E-2</v>
       </c>
       <c r="U131">
@@ -11651,19 +11651,19 @@
         <v>61</v>
       </c>
       <c r="AH131">
-        <f t="shared" ref="AH131" si="69">Y131-AB131-AE131</f>
+        <f t="shared" si="27"/>
         <v>77</v>
       </c>
       <c r="AI131">
-        <f t="shared" ref="AI131" si="70">Z131-AC131-AF131</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ131">
-        <f t="shared" ref="AJ131" si="71">AA131-AD131-AG131</f>
+        <f t="shared" si="29"/>
         <v>744</v>
       </c>
       <c r="AK131">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
     </row>
@@ -11715,15 +11715,15 @@
         <v>388</v>
       </c>
       <c r="R132">
-        <f t="shared" ref="R132" si="72">M132-M131</f>
+        <f t="shared" si="25"/>
         <v>3698</v>
       </c>
       <c r="S132" s="8">
-        <f t="shared" ref="S132" si="73">Q132/U132</f>
+        <f t="shared" si="26"/>
         <v>9.4958394517865877E-2</v>
       </c>
       <c r="T132" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>9.3702497285559169E-2</v>
       </c>
       <c r="U132">
@@ -11770,19 +11770,19 @@
         <v>61</v>
       </c>
       <c r="AH132">
-        <f t="shared" ref="AH132" si="74">Y132-AB132-AE132</f>
+        <f t="shared" si="27"/>
         <v>80</v>
       </c>
       <c r="AI132">
-        <f t="shared" ref="AI132" si="75">Z132-AC132-AF132</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ132">
-        <f t="shared" ref="AJ132" si="76">AA132-AD132-AG132</f>
+        <f t="shared" si="29"/>
         <v>758</v>
       </c>
       <c r="AK132">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
     </row>
@@ -11822,43 +11822,43 @@
         <v>7</v>
       </c>
       <c r="M133" s="7">
-        <f t="shared" ref="M133:M150" si="77">B133-C133</f>
+        <f t="shared" ref="M133:M150" si="32">B133-C133</f>
         <v>413315</v>
       </c>
       <c r="N133" s="4">
-        <f t="shared" ref="N133:N150" si="78">C133/B133</f>
+        <f t="shared" ref="N133:N150" si="33">C133/B133</f>
         <v>9.3084388583766511E-2</v>
       </c>
       <c r="Q133">
-        <f t="shared" ref="Q133:Q150" si="79">C133-C132</f>
+        <f t="shared" ref="Q133:Q150" si="34">C133-C132</f>
         <v>406</v>
       </c>
       <c r="R133">
-        <f t="shared" ref="R133" si="80">M133-M132</f>
+        <f t="shared" si="25"/>
         <v>3994</v>
       </c>
       <c r="S133" s="8">
-        <f t="shared" ref="S133" si="81">Q133/U133</f>
+        <f t="shared" si="26"/>
         <v>9.227272727272727E-2</v>
       </c>
       <c r="T133" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="30"/>
         <v>9.6380586783657796E-2</v>
       </c>
       <c r="U133">
-        <f t="shared" ref="U133:U150" si="82">B133-B132</f>
+        <f t="shared" ref="U133:U150" si="35">B133-B132</f>
         <v>4400</v>
       </c>
       <c r="V133">
-        <f t="shared" ref="V133:V150" si="83">C133-D133-E133</f>
+        <f t="shared" ref="V133:V150" si="36">C133-D133-E133</f>
         <v>11866</v>
       </c>
       <c r="W133" s="3">
-        <f t="shared" ref="W133:W150" si="84">F133/V133</f>
+        <f t="shared" ref="W133:W150" si="37">F133/V133</f>
         <v>2.0310129782572055E-2</v>
       </c>
       <c r="X133">
-        <f t="shared" ref="X133:X150" si="85">E133-E132</f>
+        <f t="shared" ref="X133:X150" si="38">E133-E132</f>
         <v>3</v>
       </c>
       <c r="Y133">
@@ -11889,19 +11889,19 @@
         <v>61</v>
       </c>
       <c r="AH133">
-        <f t="shared" ref="AH133" si="86">Y133-AB133-AE133</f>
+        <f t="shared" si="27"/>
         <v>78</v>
       </c>
       <c r="AI133">
-        <f t="shared" ref="AI133" si="87">Z133-AC133-AF133</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ133">
-        <f t="shared" ref="AJ133" si="88">AA133-AD133-AG133</f>
+        <f t="shared" si="29"/>
         <v>764</v>
       </c>
       <c r="AK133">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
     </row>
@@ -11941,43 +11941,43 @@
         <v>5</v>
       </c>
       <c r="M134" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>416054</v>
       </c>
       <c r="N134" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3153324382290889E-2</v>
       </c>
       <c r="Q134">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>316</v>
       </c>
       <c r="R134">
-        <f t="shared" ref="R134" si="89">M134-M133</f>
+        <f t="shared" si="25"/>
         <v>2739</v>
       </c>
       <c r="S134" s="8">
-        <f t="shared" ref="S134" si="90">Q134/U134</f>
+        <f t="shared" si="26"/>
         <v>0.10343698854337152</v>
       </c>
       <c r="T134" s="8">
-        <f t="shared" ref="T134" si="91">SUM(Q128:Q134)/SUM(U128:U134)</f>
+        <f t="shared" ref="T134:T172" si="39">SUM(Q128:Q134)/SUM(U128:U134)</f>
         <v>9.3306345056366147E-2</v>
       </c>
       <c r="U134">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>3055</v>
       </c>
       <c r="V134">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11426</v>
       </c>
       <c r="W134" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.2142482058463153E-2</v>
       </c>
       <c r="X134">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="Y134">
@@ -12008,19 +12008,19 @@
         <v>62</v>
       </c>
       <c r="AH134">
-        <f t="shared" ref="AH134" si="92">Y134-AB134-AE134</f>
+        <f t="shared" si="27"/>
         <v>80</v>
       </c>
       <c r="AI134">
-        <f t="shared" ref="AI134" si="93">Z134-AC134-AF134</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AJ134">
-        <f t="shared" ref="AJ134" si="94">AA134-AD134-AG134</f>
+        <f t="shared" si="29"/>
         <v>770</v>
       </c>
       <c r="AK134">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
     </row>
@@ -12060,43 +12060,43 @@
         <v>5</v>
       </c>
       <c r="M135" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>420769</v>
       </c>
       <c r="N135" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3099895681561504E-2</v>
       </c>
       <c r="Q135">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>457</v>
       </c>
       <c r="R135">
-        <f t="shared" ref="R135" si="95">M135-M134</f>
+        <f t="shared" si="25"/>
         <v>4715</v>
       </c>
       <c r="S135" s="8">
-        <f t="shared" ref="S135" si="96">Q135/U135</f>
+        <f t="shared" si="26"/>
         <v>8.8360402165506571E-2</v>
       </c>
       <c r="T135" s="8">
-        <f t="shared" ref="T135" si="97">SUM(Q129:Q135)/SUM(U129:U135)</f>
+        <f t="shared" si="39"/>
         <v>9.4353228311515422E-2</v>
       </c>
       <c r="U135">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5172</v>
       </c>
       <c r="V135">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11137</v>
       </c>
       <c r="W135" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.2088533716440692E-2</v>
       </c>
       <c r="X135">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="Y135">
@@ -12127,19 +12127,19 @@
         <v>62</v>
       </c>
       <c r="AH135">
-        <f t="shared" ref="AH135" si="98">Y135-AB135-AE135</f>
+        <f t="shared" si="27"/>
         <v>79</v>
       </c>
       <c r="AI135">
-        <f t="shared" ref="AI135" si="99">Z135-AC135-AF135</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ135">
-        <f t="shared" ref="AJ135" si="100">AA135-AD135-AG135</f>
+        <f t="shared" si="29"/>
         <v>754</v>
       </c>
       <c r="AK135">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
     </row>
@@ -12179,43 +12179,43 @@
         <v>7</v>
       </c>
       <c r="M136" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>425833</v>
       </c>
       <c r="N136" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3129143480214588E-2</v>
       </c>
       <c r="Q136">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>535</v>
       </c>
       <c r="R136">
-        <f t="shared" ref="R136" si="101">M136-M135</f>
+        <f t="shared" si="25"/>
         <v>5064</v>
       </c>
       <c r="S136" s="8">
-        <f t="shared" ref="S136" si="102">Q136/U136</f>
+        <f t="shared" si="26"/>
         <v>9.5552777281657439E-2</v>
       </c>
       <c r="T136" s="8">
-        <f t="shared" ref="T136" si="103">SUM(Q130:Q136)/SUM(U130:U136)</f>
+        <f t="shared" si="39"/>
         <v>9.8114471960766392E-2</v>
       </c>
       <c r="U136">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5599</v>
       </c>
       <c r="V136">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11140</v>
       </c>
       <c r="W136" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.1274685816876124E-2</v>
       </c>
       <c r="X136">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>10</v>
       </c>
       <c r="Y136">
@@ -12246,19 +12246,19 @@
         <v>62</v>
       </c>
       <c r="AH136">
-        <f t="shared" ref="AH136" si="104">Y136-AB136-AE136</f>
+        <f t="shared" si="27"/>
         <v>80</v>
       </c>
       <c r="AI136">
-        <f t="shared" ref="AI136" si="105">Z136-AC136-AF136</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ136">
-        <f t="shared" ref="AJ136" si="106">AA136-AD136-AG136</f>
+        <f t="shared" si="29"/>
         <v>714</v>
       </c>
       <c r="AK136">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>11</v>
       </c>
     </row>
@@ -12298,43 +12298,43 @@
         <v>5</v>
       </c>
       <c r="M137" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>431023</v>
       </c>
       <c r="N137" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3531610083764982E-2</v>
       </c>
       <c r="Q137">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>744</v>
       </c>
       <c r="R137">
-        <f t="shared" ref="R137" si="107">M137-M136</f>
+        <f t="shared" si="25"/>
         <v>5190</v>
       </c>
       <c r="S137" s="8">
-        <f t="shared" ref="S137" si="108">Q137/U137</f>
+        <f t="shared" si="26"/>
         <v>0.12537917087967643</v>
       </c>
       <c r="T137" s="8">
-        <f t="shared" ref="T137" si="109">SUM(Q131:Q137)/SUM(U131:U137)</f>
+        <f t="shared" si="39"/>
         <v>0.10262550743261004</v>
       </c>
       <c r="U137">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5934</v>
       </c>
       <c r="V137">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11114</v>
       </c>
       <c r="W137" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.0244736368544177E-2</v>
       </c>
       <c r="X137">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>11</v>
       </c>
       <c r="Y137">
@@ -12365,19 +12365,19 @@
         <v>62</v>
       </c>
       <c r="AH137">
-        <f t="shared" ref="AH137" si="110">Y137-AB137-AE137</f>
+        <f t="shared" si="27"/>
         <v>84</v>
       </c>
       <c r="AI137">
-        <f t="shared" ref="AI137" si="111">Z137-AC137-AF137</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AJ137">
-        <f t="shared" ref="AJ137" si="112">AA137-AD137-AG137</f>
+        <f t="shared" si="29"/>
         <v>710</v>
       </c>
       <c r="AK137">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
     </row>
@@ -12417,43 +12417,43 @@
         <v>9</v>
       </c>
       <c r="M138" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>435488</v>
       </c>
       <c r="N138" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.353593172711662E-2</v>
       </c>
       <c r="Q138">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>463</v>
       </c>
       <c r="R138">
-        <f t="shared" ref="R138:R140" si="113">M138-M137</f>
+        <f t="shared" si="25"/>
         <v>4465</v>
       </c>
       <c r="S138" s="8">
-        <f t="shared" ref="S138:S140" si="114">Q138/U138</f>
+        <f t="shared" si="26"/>
         <v>9.395292207792208E-2</v>
       </c>
       <c r="T138" s="8">
-        <f t="shared" ref="T138:T140" si="115">SUM(Q132:Q138)/SUM(U132:U138)</f>
+        <f t="shared" si="39"/>
         <v>9.9746789654548737E-2</v>
       </c>
       <c r="U138">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>4928</v>
       </c>
       <c r="V138">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11263</v>
       </c>
       <c r="W138" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.1486282517979224E-2</v>
       </c>
       <c r="X138">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="Y138">
@@ -12484,19 +12484,19 @@
         <v>62</v>
       </c>
       <c r="AH138">
-        <f t="shared" ref="AH138:AH139" si="116">Y138-AB138-AE138</f>
+        <f t="shared" si="27"/>
         <v>85</v>
       </c>
       <c r="AI138">
-        <f t="shared" ref="AI138:AI139" si="117">Z138-AC138-AF138</f>
+        <f t="shared" si="28"/>
         <v>20</v>
       </c>
       <c r="AJ138">
-        <f t="shared" ref="AJ138:AJ139" si="118">AA138-AD138-AG138</f>
+        <f t="shared" si="29"/>
         <v>663</v>
       </c>
       <c r="AK138">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
     </row>
@@ -12536,43 +12536,43 @@
         <v>7</v>
       </c>
       <c r="M139" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>440348</v>
       </c>
       <c r="N139" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3613377573956214E-2</v>
       </c>
       <c r="Q139">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>543</v>
       </c>
       <c r="R139">
-        <f t="shared" si="113"/>
+        <f t="shared" si="25"/>
         <v>4860</v>
       </c>
       <c r="S139" s="8">
-        <f t="shared" si="114"/>
+        <f t="shared" si="26"/>
         <v>0.10049972237645752</v>
       </c>
       <c r="T139" s="8">
-        <f t="shared" si="115"/>
+        <f t="shared" si="39"/>
         <v>0.10043199675277609</v>
       </c>
       <c r="U139">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5403</v>
       </c>
       <c r="V139">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11689</v>
       </c>
       <c r="W139" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>1.9762169561125843E-2</v>
       </c>
       <c r="X139">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="Y139">
@@ -12603,19 +12603,19 @@
         <v>62</v>
       </c>
       <c r="AH139">
-        <f t="shared" si="116"/>
+        <f t="shared" si="27"/>
         <v>89</v>
       </c>
       <c r="AI139">
-        <f t="shared" si="117"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ139">
-        <f t="shared" si="118"/>
+        <f t="shared" si="29"/>
         <v>672</v>
       </c>
       <c r="AK139">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
     </row>
@@ -12655,43 +12655,43 @@
         <v>7</v>
       </c>
       <c r="M140" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>442356</v>
       </c>
       <c r="N140" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3789051456760184E-2</v>
       </c>
       <c r="Q140">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>302</v>
       </c>
       <c r="R140">
-        <f t="shared" si="113"/>
+        <f t="shared" si="25"/>
         <v>2008</v>
       </c>
       <c r="S140" s="8">
-        <f t="shared" si="114"/>
+        <f t="shared" si="26"/>
         <v>0.13073593073593073</v>
       </c>
       <c r="T140" s="8">
-        <f t="shared" si="115"/>
+        <f t="shared" si="39"/>
         <v>0.10370050307089287</v>
       </c>
       <c r="U140">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>2310</v>
       </c>
       <c r="V140">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11802</v>
       </c>
       <c r="W140" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.0420267751228606E-2</v>
       </c>
       <c r="X140">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="Y140">
@@ -12722,19 +12722,19 @@
         <v>62</v>
       </c>
       <c r="AH140">
-        <f t="shared" ref="AH140" si="119">Y140-AB140-AE140</f>
+        <f t="shared" si="27"/>
         <v>88</v>
       </c>
       <c r="AI140">
-        <f t="shared" ref="AI140" si="120">Z140-AC140-AF140</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ140">
-        <f t="shared" ref="AJ140" si="121">AA140-AD140-AG140</f>
+        <f t="shared" si="29"/>
         <v>676</v>
       </c>
       <c r="AK140">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
     </row>
@@ -12774,43 +12774,43 @@
         <v>6</v>
       </c>
       <c r="M141" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>445947</v>
       </c>
       <c r="N141" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3472838560036103E-2</v>
       </c>
       <c r="Q141">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>200</v>
       </c>
       <c r="R141">
-        <f t="shared" ref="R141" si="122">M141-M140</f>
+        <f t="shared" si="25"/>
         <v>3591</v>
       </c>
       <c r="S141" s="8">
-        <f t="shared" ref="S141" si="123">Q141/U141</f>
+        <f t="shared" si="26"/>
         <v>5.2756528620416777E-2</v>
       </c>
       <c r="T141" s="8">
-        <f t="shared" ref="T141" si="124">SUM(Q135:Q141)/SUM(U135:U141)</f>
+        <f t="shared" si="39"/>
         <v>9.7896611039019824E-2</v>
       </c>
       <c r="U141">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>3791</v>
       </c>
       <c r="V141">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>11174</v>
       </c>
       <c r="W141" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.1746912475389298E-2</v>
       </c>
       <c r="X141">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="Y141">
@@ -12841,19 +12841,19 @@
         <v>62</v>
       </c>
       <c r="AH141">
-        <f t="shared" ref="AH141" si="125">Y141-AB141-AE141</f>
+        <f t="shared" si="27"/>
         <v>89</v>
       </c>
       <c r="AI141">
-        <f t="shared" ref="AI141" si="126">Z141-AC141-AF141</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AJ141">
-        <f t="shared" ref="AJ141" si="127">AA141-AD141-AG141</f>
+        <f t="shared" si="29"/>
         <v>619</v>
       </c>
       <c r="AK141">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>12</v>
       </c>
     </row>
@@ -12893,43 +12893,43 @@
         <v>8</v>
       </c>
       <c r="M142" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>450768</v>
       </c>
       <c r="N142" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.335049680196307E-2</v>
       </c>
       <c r="Q142">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>430</v>
       </c>
       <c r="R142">
-        <f t="shared" ref="R142" si="128">M142-M141</f>
+        <f t="shared" si="25"/>
         <v>4821</v>
       </c>
       <c r="S142" s="8">
-        <f t="shared" ref="S142" si="129">Q142/U142</f>
+        <f t="shared" si="26"/>
         <v>8.1889163968767859E-2</v>
       </c>
       <c r="T142" s="8">
-        <f t="shared" ref="T142" si="130">SUM(Q136:Q142)/SUM(U136:U142)</f>
+        <f t="shared" si="39"/>
         <v>9.6850915221579958E-2</v>
       </c>
       <c r="U142">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5251</v>
       </c>
       <c r="V142">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10860</v>
       </c>
       <c r="W142" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.2836095764272559E-2</v>
       </c>
       <c r="X142">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="Y142">
@@ -12960,19 +12960,19 @@
         <v>62</v>
       </c>
       <c r="AH142">
-        <f t="shared" ref="AH142" si="131">Y142-AB142-AE142</f>
+        <f t="shared" si="27"/>
         <v>83</v>
       </c>
       <c r="AI142">
-        <f t="shared" ref="AI142" si="132">Z142-AC142-AF142</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="AJ142">
-        <f t="shared" ref="AJ142" si="133">AA142-AD142-AG142</f>
+        <f t="shared" si="29"/>
         <v>593</v>
       </c>
       <c r="AK142">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13012,43 +13012,43 @@
         <v>9</v>
       </c>
       <c r="M143" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>456637</v>
       </c>
       <c r="N143" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.335718554492442E-2</v>
       </c>
       <c r="Q143">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>608</v>
       </c>
       <c r="R143">
-        <f t="shared" ref="R143" si="134">M143-M142</f>
+        <f t="shared" si="25"/>
         <v>5869</v>
       </c>
       <c r="S143" s="8">
-        <f t="shared" ref="S143" si="135">Q143/U143</f>
+        <f t="shared" si="26"/>
         <v>9.3870619113787246E-2</v>
       </c>
       <c r="T143" s="8">
-        <f t="shared" ref="T143" si="136">SUM(Q137:Q143)/SUM(U137:U143)</f>
+        <f t="shared" si="39"/>
         <v>9.6497917522144663E-2</v>
       </c>
       <c r="U143">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>6477</v>
       </c>
       <c r="V143">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10646</v>
       </c>
       <c r="W143" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.2261882397144467E-2</v>
       </c>
       <c r="X143">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>13</v>
       </c>
       <c r="Y143">
@@ -13079,19 +13079,19 @@
         <v>62</v>
       </c>
       <c r="AH143">
-        <f t="shared" ref="AH143" si="137">Y143-AB143-AE143</f>
+        <f t="shared" si="27"/>
         <v>86</v>
       </c>
       <c r="AI143">
-        <f t="shared" ref="AI143" si="138">Z143-AC143-AF143</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ143">
-        <f t="shared" ref="AJ143" si="139">AA143-AD143-AG143</f>
+        <f t="shared" si="29"/>
         <v>579</v>
       </c>
       <c r="AK143">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>7</v>
       </c>
     </row>
@@ -13131,43 +13131,43 @@
         <v>9</v>
       </c>
       <c r="M144" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>462794</v>
       </c>
       <c r="N144" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3488625367760841E-2</v>
       </c>
       <c r="Q144">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>708</v>
       </c>
       <c r="R144">
-        <f t="shared" ref="R144" si="140">M144-M143</f>
+        <f t="shared" si="25"/>
         <v>6157</v>
       </c>
       <c r="S144" s="8">
-        <f t="shared" ref="S144" si="141">Q144/U144</f>
+        <f t="shared" si="26"/>
         <v>0.10313182811361982</v>
       </c>
       <c r="T144" s="8">
-        <f t="shared" ref="T144" si="142">SUM(Q138:Q144)/SUM(U138:U144)</f>
+        <f t="shared" si="39"/>
         <v>9.2905067808708067E-2</v>
       </c>
       <c r="U144">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>6865</v>
       </c>
       <c r="V144">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10568</v>
       </c>
       <c r="W144" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.1101438304314914E-2</v>
       </c>
       <c r="X144">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>6</v>
       </c>
       <c r="Y144">
@@ -13198,19 +13198,19 @@
         <v>63</v>
       </c>
       <c r="AH144">
-        <f t="shared" ref="AH144" si="143">Y144-AB144-AE144</f>
+        <f t="shared" si="27"/>
         <v>91</v>
       </c>
       <c r="AI144">
-        <f t="shared" ref="AI144" si="144">Z144-AC144-AF144</f>
+        <f t="shared" si="28"/>
         <v>14</v>
       </c>
       <c r="AJ144">
-        <f t="shared" ref="AJ144" si="145">AA144-AD144-AG144</f>
+        <f t="shared" si="29"/>
         <v>569</v>
       </c>
       <c r="AK144">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>12</v>
       </c>
     </row>
@@ -13250,43 +13250,43 @@
         <v>7</v>
       </c>
       <c r="M145" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>466339</v>
       </c>
       <c r="N145" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3521054483322999E-2</v>
       </c>
       <c r="Q145">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>384</v>
       </c>
       <c r="R145">
-        <f t="shared" ref="R145" si="146">M145-M144</f>
+        <f t="shared" si="25"/>
         <v>3545</v>
       </c>
       <c r="S145" s="8">
-        <f t="shared" ref="S145" si="147">Q145/U145</f>
+        <f t="shared" si="26"/>
         <v>9.7734792568083484E-2</v>
       </c>
       <c r="T145" s="8">
-        <f t="shared" ref="T145" si="148">SUM(Q139:Q145)/SUM(U139:U145)</f>
+        <f t="shared" si="39"/>
         <v>9.3310997472521015E-2</v>
       </c>
       <c r="U145">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>3929</v>
       </c>
       <c r="V145">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10337</v>
       </c>
       <c r="W145" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.2153429428267389E-2</v>
       </c>
       <c r="X145">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>13</v>
       </c>
       <c r="Y145">
@@ -13317,19 +13317,19 @@
         <v>66</v>
       </c>
       <c r="AH145">
-        <f t="shared" ref="AH145" si="149">Y145-AB145-AE145</f>
+        <f t="shared" si="27"/>
         <v>97</v>
       </c>
       <c r="AI145">
-        <f t="shared" ref="AI145" si="150">Z145-AC145-AF145</f>
+        <f t="shared" si="28"/>
         <v>13</v>
       </c>
       <c r="AJ145">
-        <f t="shared" ref="AJ145" si="151">AA145-AD145-AG145</f>
+        <f t="shared" si="29"/>
         <v>549</v>
       </c>
       <c r="AK145">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
     </row>
@@ -13369,43 +13369,43 @@
         <v>10</v>
       </c>
       <c r="M146" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>472650</v>
       </c>
       <c r="N146" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3466978146541313E-2</v>
       </c>
       <c r="Q146">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>620</v>
       </c>
       <c r="R146">
-        <f t="shared" ref="R146" si="152">M146-M145</f>
+        <f t="shared" si="25"/>
         <v>6311</v>
       </c>
       <c r="S146" s="8">
-        <f t="shared" ref="S146" si="153">Q146/U146</f>
+        <f t="shared" si="26"/>
         <v>8.9453181359111233E-2</v>
       </c>
       <c r="T146" s="8">
-        <f t="shared" ref="T146" si="154">SUM(Q140:Q146)/SUM(U140:U146)</f>
+        <f t="shared" si="39"/>
         <v>9.1466501659447599E-2</v>
       </c>
       <c r="U146">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>6931</v>
       </c>
       <c r="V146">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10716</v>
       </c>
       <c r="W146" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.0623366927958194E-2</v>
       </c>
       <c r="X146">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>5</v>
       </c>
       <c r="Y146">
@@ -13436,19 +13436,19 @@
         <v>66</v>
       </c>
       <c r="AH146">
-        <f t="shared" ref="AH146" si="155">Y146-AB146-AE146</f>
+        <f t="shared" si="27"/>
         <v>108</v>
       </c>
       <c r="AI146">
-        <f t="shared" ref="AI146" si="156">Z146-AC146-AF146</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ146">
-        <f t="shared" ref="AJ146" si="157">AA146-AD146-AG146</f>
+        <f t="shared" si="29"/>
         <v>563</v>
       </c>
       <c r="AK146">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>12</v>
       </c>
     </row>
@@ -13488,43 +13488,43 @@
         <v>7</v>
       </c>
       <c r="M147" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>474928</v>
       </c>
       <c r="N147" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3524301048999101E-2</v>
       </c>
       <c r="Q147">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>268</v>
       </c>
       <c r="R147">
-        <f t="shared" ref="R147" si="158">M147-M146</f>
+        <f t="shared" si="25"/>
         <v>2278</v>
       </c>
       <c r="S147" s="8">
-        <f t="shared" ref="S147" si="159">Q147/U147</f>
+        <f t="shared" si="26"/>
         <v>0.10526315789473684</v>
       </c>
       <c r="T147" s="8">
-        <f t="shared" ref="T147" si="160">SUM(Q141:Q147)/SUM(U141:U147)</f>
+        <f t="shared" si="39"/>
         <v>8.9913383626711377E-2</v>
       </c>
       <c r="U147">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>2546</v>
       </c>
       <c r="V147">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10822</v>
       </c>
       <c r="W147" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.0698576972833119E-2</v>
       </c>
       <c r="X147">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="Y147">
@@ -13555,19 +13555,19 @@
         <v>66</v>
       </c>
       <c r="AH147">
-        <f t="shared" ref="AH147" si="161">Y147-AB147-AE147</f>
+        <f t="shared" si="27"/>
         <v>106</v>
       </c>
       <c r="AI147">
-        <f t="shared" ref="AI147" si="162">Z147-AC147-AF147</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ147">
-        <f t="shared" ref="AJ147" si="163">AA147-AD147-AG147</f>
+        <f t="shared" si="29"/>
         <v>559</v>
       </c>
       <c r="AK147">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
     </row>
@@ -13607,43 +13607,43 @@
         <v>10</v>
       </c>
       <c r="M148" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>476429</v>
       </c>
       <c r="N148" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3540058562423783E-2</v>
       </c>
       <c r="Q148">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>164</v>
       </c>
       <c r="R148">
-        <f t="shared" ref="R148" si="164">M148-M147</f>
+        <f t="shared" si="25"/>
         <v>1501</v>
       </c>
       <c r="S148" s="8">
-        <f t="shared" ref="S148" si="165">Q148/U148</f>
+        <f t="shared" si="26"/>
         <v>9.8498498498498496E-2</v>
       </c>
       <c r="T148" s="8">
-        <f t="shared" ref="T148" si="166">SUM(Q142:Q148)/SUM(U142:U148)</f>
+        <f t="shared" si="39"/>
         <v>9.452233840304182E-2</v>
       </c>
       <c r="U148">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>1665</v>
       </c>
       <c r="V148">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10250</v>
       </c>
       <c r="W148" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.3804878048780488E-2</v>
       </c>
       <c r="X148">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="Y148">
@@ -13674,19 +13674,19 @@
         <v>66</v>
       </c>
       <c r="AH148">
-        <f t="shared" ref="AH148" si="167">Y148-AB148-AE148</f>
+        <f t="shared" si="27"/>
         <v>104</v>
       </c>
       <c r="AI148">
-        <f t="shared" ref="AI148" si="168">Z148-AC148-AF148</f>
+        <f t="shared" si="28"/>
         <v>13</v>
       </c>
       <c r="AJ148">
-        <f t="shared" ref="AJ148" si="169">AA148-AD148-AG148</f>
+        <f t="shared" si="29"/>
         <v>535</v>
       </c>
       <c r="AK148">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="AL148">
@@ -13735,43 +13735,43 @@
         <v>4</v>
       </c>
       <c r="M149" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>480810</v>
       </c>
       <c r="N149" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3509147674997364E-2</v>
       </c>
       <c r="Q149">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>434</v>
       </c>
       <c r="R149">
-        <f t="shared" ref="R149" si="170">M149-M148</f>
+        <f t="shared" si="25"/>
         <v>4381</v>
       </c>
       <c r="S149" s="8">
-        <f t="shared" ref="S149" si="171">Q149/U149</f>
+        <f t="shared" si="26"/>
         <v>9.0134994807891999E-2</v>
       </c>
       <c r="T149" s="8">
-        <f t="shared" ref="T149" si="172">SUM(Q143:Q149)/SUM(U143:U149)</f>
+        <f t="shared" si="39"/>
         <v>9.5882990249187436E-2</v>
       </c>
       <c r="U149">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>4815</v>
       </c>
       <c r="V149">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>10121</v>
       </c>
       <c r="W149" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.4009485228732339E-2</v>
       </c>
       <c r="X149">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>11</v>
       </c>
       <c r="Y149">
@@ -13802,19 +13802,19 @@
         <v>66</v>
       </c>
       <c r="AH149">
-        <f t="shared" ref="AH149" si="173">Y149-AB149-AE149</f>
+        <f t="shared" si="27"/>
         <v>103</v>
       </c>
       <c r="AI149">
-        <f t="shared" ref="AI149" si="174">Z149-AC149-AF149</f>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="AJ149">
-        <f t="shared" ref="AJ149" si="175">AA149-AD149-AG149</f>
+        <f t="shared" si="29"/>
         <v>529</v>
       </c>
       <c r="AK149">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="AL149">
@@ -13863,43 +13863,43 @@
         <v>8</v>
       </c>
       <c r="M150" s="7">
-        <f t="shared" si="77"/>
+        <f t="shared" si="32"/>
         <v>485882</v>
       </c>
       <c r="N150" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="33"/>
         <v>9.3309198801981769E-2</v>
       </c>
       <c r="Q150">
-        <f t="shared" si="79"/>
+        <f t="shared" si="34"/>
         <v>405</v>
       </c>
       <c r="R150">
-        <f t="shared" ref="R150" si="176">M150-M149</f>
+        <f t="shared" si="25"/>
         <v>5072</v>
       </c>
       <c r="S150" s="8">
-        <f t="shared" ref="S150" si="177">Q150/U150</f>
+        <f t="shared" si="26"/>
         <v>7.3945590651816689E-2</v>
       </c>
       <c r="T150" s="8">
-        <f t="shared" ref="T150" si="178">SUM(Q144:Q150)/SUM(U144:U150)</f>
+        <f t="shared" si="39"/>
         <v>9.2559265235199209E-2</v>
       </c>
       <c r="U150">
-        <f t="shared" si="82"/>
+        <f t="shared" si="35"/>
         <v>5477</v>
       </c>
       <c r="V150">
-        <f t="shared" si="83"/>
+        <f t="shared" si="36"/>
         <v>9808</v>
       </c>
       <c r="W150" s="3">
-        <f t="shared" si="84"/>
+        <f t="shared" si="37"/>
         <v>2.6610929853181076E-2</v>
       </c>
       <c r="X150">
-        <f t="shared" si="85"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="Y150">
@@ -13930,19 +13930,19 @@
         <v>66</v>
       </c>
       <c r="AH150">
-        <f t="shared" ref="AH150" si="179">Y150-AB150-AE150</f>
+        <f t="shared" si="27"/>
         <v>101</v>
       </c>
       <c r="AI150">
-        <f t="shared" ref="AI150" si="180">Z150-AC150-AF150</f>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="AJ150">
-        <f t="shared" ref="AJ150" si="181">AA150-AD150-AG150</f>
+        <f t="shared" si="29"/>
         <v>525</v>
       </c>
       <c r="AK150">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
     </row>
@@ -13982,43 +13982,43 @@
         <v>12</v>
       </c>
       <c r="M151" s="7">
-        <f t="shared" ref="M151:M157" si="182">B151-C151</f>
+        <f t="shared" ref="M151:M157" si="40">B151-C151</f>
         <v>490293</v>
       </c>
       <c r="N151" s="4">
-        <f t="shared" ref="N151:N156" si="183">C151/B151</f>
+        <f t="shared" ref="N151:N156" si="41">C151/B151</f>
         <v>9.3684724219648269E-2</v>
       </c>
       <c r="Q151">
-        <f t="shared" ref="Q151:Q153" si="184">C151-C150</f>
+        <f t="shared" ref="Q151:Q172" si="42">C151-C150</f>
         <v>678</v>
       </c>
       <c r="R151">
-        <f t="shared" ref="R151:R153" si="185">M151-M150</f>
+        <f t="shared" si="25"/>
         <v>4411</v>
       </c>
       <c r="S151" s="8">
-        <f t="shared" ref="S151:S153" si="186">Q151/U151</f>
+        <f t="shared" si="26"/>
         <v>0.13322853212811947</v>
       </c>
       <c r="T151" s="8">
-        <f t="shared" ref="T151:T153" si="187">SUM(Q145:Q151)/SUM(U145:U151)</f>
+        <f t="shared" si="39"/>
         <v>9.697228425062393E-2</v>
       </c>
       <c r="U151">
-        <f t="shared" ref="U151:U153" si="188">B151-B150</f>
+        <f t="shared" ref="U151:U172" si="43">B151-B150</f>
         <v>5089</v>
       </c>
       <c r="V151">
-        <f t="shared" ref="V151:V153" si="189">C151-D151-E151</f>
+        <f t="shared" ref="V151:V173" si="44">C151-D151-E151</f>
         <v>9929</v>
       </c>
       <c r="W151" s="3">
-        <f t="shared" ref="W151:W153" si="190">F151/V151</f>
+        <f t="shared" ref="W151:W173" si="45">F151/V151</f>
         <v>2.5984489878134755E-2</v>
       </c>
       <c r="X151">
-        <f t="shared" ref="X151:X153" si="191">E151-E150</f>
+        <f t="shared" ref="X151:X173" si="46">E151-E150</f>
         <v>10</v>
       </c>
       <c r="Y151">
@@ -14049,19 +14049,19 @@
         <v>66</v>
       </c>
       <c r="AH151">
-        <f t="shared" ref="AH151:AH153" si="192">Y151-AB151-AE151</f>
+        <f t="shared" si="27"/>
         <v>101</v>
       </c>
       <c r="AI151">
-        <f t="shared" ref="AI151:AI153" si="193">Z151-AC151-AF151</f>
+        <f t="shared" si="28"/>
         <v>19</v>
       </c>
       <c r="AJ151">
-        <f t="shared" ref="AJ151:AJ153" si="194">AA151-AD151-AG151</f>
+        <f t="shared" si="29"/>
         <v>539</v>
       </c>
       <c r="AK151">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="AL151">
@@ -14076,7 +14076,7 @@
     </row>
     <row r="152" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
-        <f t="shared" ref="A152:A171" si="195">A151+1</f>
+        <f t="shared" ref="A152:A173" si="47">A151+1</f>
         <v>44058</v>
       </c>
       <c r="B152">
@@ -14110,43 +14110,43 @@
         <v>11</v>
       </c>
       <c r="M152" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>500769</v>
       </c>
       <c r="N152" s="4">
-        <f t="shared" si="183"/>
+        <f t="shared" si="41"/>
         <v>9.3494588327296221E-2</v>
       </c>
       <c r="Q152">
-        <f t="shared" si="184"/>
+        <f t="shared" si="42"/>
         <v>967</v>
       </c>
       <c r="R152">
-        <f t="shared" si="185"/>
+        <f t="shared" si="25"/>
         <v>10476</v>
       </c>
       <c r="S152" s="8">
-        <f t="shared" si="186"/>
+        <f t="shared" si="26"/>
         <v>8.4505811413090978E-2</v>
       </c>
       <c r="T152" s="8">
-        <f t="shared" si="187"/>
+        <f t="shared" si="39"/>
         <v>9.3135963757045775E-2</v>
       </c>
       <c r="U152">
-        <f t="shared" si="188"/>
+        <f t="shared" si="43"/>
         <v>11443</v>
       </c>
       <c r="V152">
-        <f t="shared" si="189"/>
+        <f t="shared" si="44"/>
         <v>10317</v>
       </c>
       <c r="W152" s="3">
-        <f t="shared" si="190"/>
+        <f t="shared" si="45"/>
         <v>2.5298051759232335E-2</v>
       </c>
       <c r="X152">
-        <f t="shared" si="191"/>
+        <f t="shared" si="46"/>
         <v>8</v>
       </c>
       <c r="Y152">
@@ -14177,19 +14177,19 @@
         <v>66</v>
       </c>
       <c r="AH152">
-        <f t="shared" si="192"/>
+        <f t="shared" si="27"/>
         <v>103</v>
       </c>
       <c r="AI152">
-        <f t="shared" si="193"/>
+        <f t="shared" si="28"/>
         <v>18</v>
       </c>
       <c r="AJ152">
-        <f t="shared" si="194"/>
+        <f t="shared" si="29"/>
         <v>551</v>
       </c>
       <c r="AK152">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="AL152">
@@ -14204,7 +14204,7 @@
     </row>
     <row r="153" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44059</v>
       </c>
       <c r="B153">
@@ -14238,43 +14238,43 @@
         <v>13</v>
       </c>
       <c r="M153" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>506453</v>
       </c>
       <c r="N153" s="4">
-        <f t="shared" si="183"/>
+        <f t="shared" si="41"/>
         <v>9.3473116701332085E-2</v>
       </c>
       <c r="Q153">
-        <f t="shared" si="184"/>
+        <f t="shared" si="42"/>
         <v>573</v>
       </c>
       <c r="R153">
-        <f t="shared" si="185"/>
+        <f t="shared" si="25"/>
         <v>5684</v>
       </c>
       <c r="S153" s="8">
-        <f t="shared" si="186"/>
+        <f t="shared" si="26"/>
         <v>9.1577433274732306E-2</v>
       </c>
       <c r="T153" s="8">
-        <f t="shared" si="187"/>
+        <f t="shared" si="39"/>
         <v>9.3558940255282635E-2</v>
       </c>
       <c r="U153">
-        <f t="shared" si="188"/>
+        <f t="shared" si="43"/>
         <v>6257</v>
       </c>
       <c r="V153">
-        <f t="shared" si="189"/>
+        <f t="shared" si="44"/>
         <v>10757</v>
       </c>
       <c r="W153" s="3">
-        <f t="shared" si="190"/>
+        <f t="shared" si="45"/>
         <v>2.5192897648043135E-2</v>
       </c>
       <c r="X153">
-        <f t="shared" si="191"/>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="Y153">
@@ -14305,25 +14305,25 @@
         <v>66</v>
       </c>
       <c r="AH153">
-        <f t="shared" si="192"/>
+        <f t="shared" si="27"/>
         <v>103</v>
       </c>
       <c r="AI153">
-        <f t="shared" si="193"/>
+        <f t="shared" si="28"/>
         <v>20</v>
       </c>
       <c r="AJ153">
-        <f t="shared" si="194"/>
+        <f t="shared" si="29"/>
         <v>568</v>
       </c>
       <c r="AK153">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>15</v>
       </c>
     </row>
     <row r="154" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44060</v>
       </c>
       <c r="B154">
@@ -14357,43 +14357,43 @@
         <v>5</v>
       </c>
       <c r="M154" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>508607</v>
       </c>
       <c r="N154" s="4">
-        <f t="shared" si="183"/>
+        <f t="shared" si="41"/>
         <v>9.3744320388868499E-2</v>
       </c>
       <c r="Q154">
-        <f t="shared" ref="Q154" si="196">C154-C153</f>
+        <f t="shared" si="42"/>
         <v>390</v>
       </c>
       <c r="R154">
-        <f t="shared" ref="R154" si="197">M154-M153</f>
+        <f t="shared" si="25"/>
         <v>2154</v>
       </c>
       <c r="S154" s="8">
-        <f t="shared" ref="S154" si="198">Q154/U154</f>
+        <f t="shared" si="26"/>
         <v>0.15330188679245282</v>
       </c>
       <c r="T154" s="8">
-        <f t="shared" ref="T154" si="199">SUM(Q148:Q154)/SUM(U148:U154)</f>
+        <f t="shared" si="39"/>
         <v>9.6835612764816309E-2</v>
       </c>
       <c r="U154">
-        <f t="shared" ref="U154" si="200">B154-B153</f>
+        <f t="shared" si="43"/>
         <v>2544</v>
       </c>
       <c r="V154">
-        <f t="shared" ref="V154" si="201">C154-D154-E154</f>
+        <f t="shared" si="44"/>
         <v>11000</v>
       </c>
       <c r="W154" s="3">
-        <f t="shared" ref="W154" si="202">F154/V154</f>
+        <f t="shared" si="45"/>
         <v>2.5727272727272727E-2</v>
       </c>
       <c r="X154">
-        <f t="shared" ref="X154" si="203">E154-E153</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Y154">
@@ -14424,19 +14424,19 @@
         <v>66</v>
       </c>
       <c r="AH154">
-        <f t="shared" ref="AH154" si="204">Y154-AB154-AE154</f>
+        <f t="shared" si="27"/>
         <v>104</v>
       </c>
       <c r="AI154">
-        <f t="shared" ref="AI154" si="205">Z154-AC154-AF154</f>
+        <f t="shared" si="28"/>
         <v>22</v>
       </c>
       <c r="AJ154">
-        <f t="shared" ref="AJ154" si="206">AA154-AD154-AG154</f>
+        <f t="shared" si="29"/>
         <v>587</v>
       </c>
       <c r="AK154">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="AL154">
@@ -14451,7 +14451,7 @@
     </row>
     <row r="155" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44061</v>
       </c>
       <c r="B155">
@@ -14485,43 +14485,43 @@
         <v>7</v>
       </c>
       <c r="M155" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>511525</v>
       </c>
       <c r="N155" s="4">
-        <f t="shared" si="183"/>
+        <f t="shared" si="41"/>
         <v>9.3752602122800704E-2</v>
       </c>
       <c r="Q155">
-        <f t="shared" ref="Q155" si="207">C155-C154</f>
+        <f t="shared" si="42"/>
         <v>307</v>
       </c>
       <c r="R155">
-        <f t="shared" ref="R155" si="208">M155-M154</f>
+        <f t="shared" ref="R155:R172" si="48">M155-M154</f>
         <v>2918</v>
       </c>
       <c r="S155" s="8">
-        <f t="shared" ref="S155" si="209">Q155/U155</f>
+        <f t="shared" ref="S155:S172" si="49">Q155/U155</f>
         <v>9.5193798449612399E-2</v>
       </c>
       <c r="T155" s="8">
-        <f t="shared" ref="T155" si="210">SUM(Q149:Q155)/SUM(U149:U155)</f>
+        <f t="shared" si="39"/>
         <v>9.6628056628056624E-2</v>
       </c>
       <c r="U155">
-        <f t="shared" ref="U155" si="211">B155-B154</f>
+        <f t="shared" si="43"/>
         <v>3225</v>
       </c>
       <c r="V155">
-        <f t="shared" ref="V155" si="212">C155-D155-E155</f>
+        <f t="shared" si="44"/>
         <v>10444</v>
       </c>
       <c r="W155" s="3">
-        <f t="shared" ref="W155" si="213">F155/V155</f>
+        <f t="shared" si="45"/>
         <v>2.7479892761394103E-2</v>
       </c>
       <c r="X155">
-        <f t="shared" ref="X155" si="214">E155-E154</f>
+        <f t="shared" si="46"/>
         <v>12</v>
       </c>
       <c r="Y155">
@@ -14552,25 +14552,25 @@
         <v>67</v>
       </c>
       <c r="AH155">
-        <f t="shared" ref="AH155" si="215">Y155-AB155-AE155</f>
+        <f t="shared" ref="AH155:AH173" si="50">Y155-AB155-AE155</f>
         <v>100</v>
       </c>
       <c r="AI155">
-        <f t="shared" ref="AI155" si="216">Z155-AC155-AF155</f>
+        <f t="shared" ref="AI155:AI173" si="51">Z155-AC155-AF155</f>
         <v>21</v>
       </c>
       <c r="AJ155">
-        <f t="shared" ref="AJ155" si="217">AA155-AD155-AG155</f>
+        <f t="shared" ref="AJ155:AJ173" si="52">AA155-AD155-AG155</f>
         <v>575</v>
       </c>
       <c r="AK155">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44062</v>
       </c>
       <c r="B156">
@@ -14604,43 +14604,43 @@
         <v>12</v>
       </c>
       <c r="M156" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>516478</v>
       </c>
       <c r="N156" s="4">
-        <f t="shared" si="183"/>
+        <f t="shared" si="41"/>
         <v>9.3836244936057023E-2</v>
       </c>
       <c r="Q156">
-        <f t="shared" ref="Q156" si="218">C156-C155</f>
+        <f t="shared" si="42"/>
         <v>565</v>
       </c>
       <c r="R156">
-        <f t="shared" ref="R156" si="219">M156-M155</f>
+        <f t="shared" si="48"/>
         <v>4953</v>
       </c>
       <c r="S156" s="8">
-        <f t="shared" ref="S156" si="220">Q156/U156</f>
+        <f t="shared" si="49"/>
         <v>0.10239217107647698</v>
       </c>
       <c r="T156" s="8">
-        <f t="shared" ref="T156" si="221">SUM(Q150:Q156)/SUM(U150:U156)</f>
+        <f t="shared" si="39"/>
         <v>9.8222637979420019E-2</v>
       </c>
       <c r="U156">
-        <f t="shared" ref="U156" si="222">B156-B155</f>
+        <f t="shared" si="43"/>
         <v>5518</v>
       </c>
       <c r="V156">
-        <f t="shared" ref="V156" si="223">C156-D156-E156</f>
+        <f t="shared" si="44"/>
         <v>10541</v>
       </c>
       <c r="W156" s="3">
-        <f t="shared" ref="W156" si="224">F156/V156</f>
+        <f t="shared" si="45"/>
         <v>2.8365430224836355E-2</v>
       </c>
       <c r="X156">
-        <f t="shared" ref="X156" si="225">E156-E155</f>
+        <f t="shared" si="46"/>
         <v>15</v>
       </c>
       <c r="Y156">
@@ -14671,19 +14671,19 @@
         <v>67</v>
       </c>
       <c r="AH156">
-        <f t="shared" ref="AH156" si="226">Y156-AB156-AE156</f>
+        <f t="shared" si="50"/>
         <v>95</v>
       </c>
       <c r="AI156">
-        <f t="shared" ref="AI156" si="227">Z156-AC156-AF156</f>
+        <f t="shared" si="51"/>
         <v>21</v>
       </c>
       <c r="AJ156">
-        <f t="shared" ref="AJ156" si="228">AA156-AD156-AG156</f>
+        <f t="shared" si="52"/>
         <v>582</v>
       </c>
       <c r="AK156">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="AL156">
@@ -14698,7 +14698,7 @@
     </row>
     <row r="157" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44063</v>
       </c>
       <c r="B157">
@@ -14732,43 +14732,43 @@
         <v>3</v>
       </c>
       <c r="M157" s="7">
-        <f t="shared" si="182"/>
+        <f t="shared" si="40"/>
         <v>522680</v>
       </c>
       <c r="N157" s="4">
-        <f t="shared" ref="N157" si="229">C157/B157</f>
+        <f>C157/B157</f>
         <v>9.3295123173987485E-2</v>
       </c>
       <c r="Q157">
-        <f t="shared" ref="Q157" si="230">C157-C156</f>
+        <f t="shared" si="42"/>
         <v>298</v>
       </c>
       <c r="R157">
-        <f t="shared" ref="R157" si="231">M157-M156</f>
+        <f t="shared" si="48"/>
         <v>6202</v>
       </c>
       <c r="S157" s="8">
-        <f t="shared" ref="S157" si="232">Q157/U157</f>
+        <f t="shared" si="49"/>
         <v>4.5846153846153849E-2</v>
       </c>
       <c r="T157" s="8">
-        <f t="shared" ref="T157" si="233">SUM(Q151:Q157)/SUM(U151:U157)</f>
+        <f t="shared" si="39"/>
         <v>9.3109227129337543E-2</v>
       </c>
       <c r="U157">
-        <f t="shared" ref="U157" si="234">B157-B156</f>
+        <f t="shared" si="43"/>
         <v>6500</v>
       </c>
       <c r="V157">
-        <f t="shared" ref="V157" si="235">C157-D157-E157</f>
+        <f t="shared" si="44"/>
         <v>10470</v>
       </c>
       <c r="W157" s="3">
-        <f t="shared" ref="W157" si="236">F157/V157</f>
+        <f t="shared" si="45"/>
         <v>2.865329512893983E-2</v>
       </c>
       <c r="X157">
-        <f t="shared" ref="X157" si="237">E157-E156</f>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
       <c r="Y157">
@@ -14799,19 +14799,19 @@
         <v>67</v>
       </c>
       <c r="AH157">
-        <f t="shared" ref="AH157" si="238">Y157-AB157-AE157</f>
+        <f t="shared" si="50"/>
         <v>95</v>
       </c>
       <c r="AI157">
-        <f t="shared" ref="AI157" si="239">Z157-AC157-AF157</f>
+        <f t="shared" si="51"/>
         <v>21</v>
       </c>
       <c r="AJ157">
-        <f t="shared" ref="AJ157" si="240">AA157-AD157-AG157</f>
+        <f t="shared" si="52"/>
         <v>588</v>
       </c>
       <c r="AK157">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="AL157">
@@ -14826,7 +14826,7 @@
     </row>
     <row r="158" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44064</v>
       </c>
       <c r="B158">
@@ -14860,43 +14860,43 @@
         <v>11</v>
       </c>
       <c r="M158" s="7">
-        <f t="shared" ref="M158:M159" si="241">B158-C158</f>
+        <f>B158-C158</f>
         <v>530839</v>
       </c>
       <c r="N158" s="4">
-        <f t="shared" ref="N158:N159" si="242">C158/B158</f>
+        <f>C158/B158</f>
         <v>9.3340780100053117E-2</v>
       </c>
       <c r="Q158">
-        <f t="shared" ref="Q158:Q159" si="243">C158-C157</f>
+        <f t="shared" si="42"/>
         <v>869</v>
       </c>
       <c r="R158">
-        <f t="shared" ref="R158:R159" si="244">M158-M157</f>
+        <f t="shared" si="48"/>
         <v>8159</v>
       </c>
       <c r="S158" s="8">
-        <f t="shared" ref="S158:S159" si="245">Q158/U158</f>
+        <f t="shared" si="49"/>
         <v>9.6256092157731496E-2</v>
       </c>
       <c r="T158" s="8">
-        <f t="shared" ref="T158:T159" si="246">SUM(Q152:Q158)/SUM(U152:U158)</f>
+        <f t="shared" si="39"/>
         <v>8.9160956980792988E-2</v>
       </c>
       <c r="U158">
-        <f t="shared" ref="U158:U159" si="247">B158-B157</f>
+        <f t="shared" si="43"/>
         <v>9028</v>
       </c>
       <c r="V158">
-        <f t="shared" ref="V158:V159" si="248">C158-D158-E158</f>
+        <f t="shared" si="44"/>
         <v>10825</v>
       </c>
       <c r="W158" s="3">
-        <f t="shared" ref="W158:W159" si="249">F158/V158</f>
+        <f t="shared" si="45"/>
         <v>2.7066974595842955E-2</v>
       </c>
       <c r="X158">
-        <f t="shared" ref="X158:X159" si="250">E158-E157</f>
+        <f t="shared" si="46"/>
         <v>5</v>
       </c>
       <c r="Y158">
@@ -14927,19 +14927,19 @@
         <v>67</v>
       </c>
       <c r="AH158">
-        <f t="shared" ref="AH158:AH159" si="251">Y158-AB158-AE158</f>
+        <f t="shared" si="50"/>
         <v>96</v>
       </c>
       <c r="AI158">
-        <f t="shared" ref="AI158:AI159" si="252">Z158-AC158-AF158</f>
+        <f t="shared" si="51"/>
         <v>19</v>
       </c>
       <c r="AJ158">
-        <f t="shared" ref="AJ158:AJ159" si="253">AA158-AD158-AG158</f>
+        <f t="shared" si="52"/>
         <v>594</v>
       </c>
       <c r="AK158">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="AL158">
@@ -14954,7 +14954,7 @@
     </row>
     <row r="159" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44065</v>
       </c>
       <c r="B159">
@@ -14988,43 +14988,43 @@
         <v>9</v>
       </c>
       <c r="M159" s="7">
-        <f t="shared" si="241"/>
+        <f>B159-C159</f>
         <v>535517</v>
       </c>
       <c r="N159" s="4">
-        <f t="shared" si="242"/>
+        <f>C159/B159</f>
         <v>9.3899795774373823E-2</v>
       </c>
       <c r="Q159">
-        <f t="shared" si="243"/>
+        <f t="shared" si="42"/>
         <v>846</v>
       </c>
       <c r="R159">
-        <f t="shared" si="244"/>
+        <f t="shared" si="48"/>
         <v>4678</v>
       </c>
       <c r="S159" s="8">
-        <f t="shared" si="245"/>
+        <f t="shared" si="49"/>
         <v>0.15314989138305576</v>
       </c>
       <c r="T159" s="8">
-        <f t="shared" si="246"/>
+        <f t="shared" si="39"/>
         <v>9.9699450720281899E-2</v>
       </c>
       <c r="U159">
-        <f t="shared" si="247"/>
+        <f t="shared" si="43"/>
         <v>5524</v>
       </c>
       <c r="V159">
-        <f t="shared" si="248"/>
+        <f t="shared" si="44"/>
         <v>11117</v>
       </c>
       <c r="W159" s="3">
-        <f t="shared" si="249"/>
+        <f t="shared" si="45"/>
         <v>2.410722317171899E-2</v>
       </c>
       <c r="X159">
-        <f t="shared" si="250"/>
+        <f t="shared" si="46"/>
         <v>14</v>
       </c>
       <c r="Y159">
@@ -15055,19 +15055,19 @@
         <v>69</v>
       </c>
       <c r="AH159">
-        <f t="shared" si="251"/>
+        <f t="shared" si="50"/>
         <v>92</v>
       </c>
       <c r="AI159">
-        <f t="shared" si="252"/>
+        <f t="shared" si="51"/>
         <v>16</v>
       </c>
       <c r="AJ159">
-        <f t="shared" si="253"/>
+        <f t="shared" si="52"/>
         <v>617</v>
       </c>
       <c r="AK159">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="AL159">
@@ -15082,7 +15082,7 @@
     </row>
     <row r="160" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44066</v>
       </c>
       <c r="B160">
@@ -15116,43 +15116,43 @@
         <v>6</v>
       </c>
       <c r="M160" s="7">
-        <f t="shared" ref="M160:M171" si="254">B160-C160</f>
+        <f t="shared" ref="M160:M171" si="53">B160-C160</f>
         <v>539169</v>
       </c>
       <c r="N160" s="4">
-        <f t="shared" ref="N160:N171" si="255">C160/B160</f>
+        <f t="shared" ref="N160:N171" si="54">C160/B160</f>
         <v>9.4223325762361074E-2</v>
       </c>
       <c r="Q160">
-        <f t="shared" ref="Q160:Q163" si="256">C160-C159</f>
+        <f t="shared" si="42"/>
         <v>591</v>
       </c>
       <c r="R160">
-        <f t="shared" ref="R160:R163" si="257">M160-M159</f>
+        <f t="shared" si="48"/>
         <v>3652</v>
       </c>
       <c r="S160" s="8">
-        <f t="shared" ref="S160:S163" si="258">Q160/U160</f>
+        <f t="shared" si="49"/>
         <v>0.13928823945321706</v>
       </c>
       <c r="T160" s="8">
-        <f t="shared" ref="T160:T163" si="259">SUM(Q154:Q160)/SUM(U154:U160)</f>
+        <f t="shared" si="39"/>
         <v>0.10568038926247882</v>
       </c>
       <c r="U160">
-        <f t="shared" ref="U160:U163" si="260">B160-B159</f>
+        <f t="shared" si="43"/>
         <v>4243</v>
       </c>
       <c r="V160">
-        <f t="shared" ref="V160:V163" si="261">C160-D160-E160</f>
+        <f t="shared" si="44"/>
         <v>11582</v>
       </c>
       <c r="W160" s="3">
-        <f t="shared" ref="W160:W163" si="262">F160/V160</f>
+        <f t="shared" si="45"/>
         <v>2.2448627180107063E-2</v>
       </c>
       <c r="X160">
-        <f t="shared" ref="X160:X163" si="263">E160-E159</f>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="Y160">
@@ -15183,19 +15183,19 @@
         <v>69</v>
       </c>
       <c r="AH160">
-        <f t="shared" ref="AH160:AH164" si="264">Y160-AB160-AE160</f>
+        <f t="shared" si="50"/>
         <v>97</v>
       </c>
       <c r="AI160">
-        <f t="shared" ref="AI160:AI164" si="265">Z160-AC160-AF160</f>
+        <f t="shared" si="51"/>
         <v>23</v>
       </c>
       <c r="AJ160">
-        <f t="shared" ref="AJ160:AJ164" si="266">AA160-AD160-AG160</f>
+        <f t="shared" si="52"/>
         <v>619</v>
       </c>
       <c r="AK160">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="AL160">
@@ -15210,7 +15210,7 @@
     </row>
     <row r="161" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44067</v>
       </c>
       <c r="B161">
@@ -15244,43 +15244,43 @@
         <v>8</v>
       </c>
       <c r="M161" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>541046</v>
       </c>
       <c r="N161" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>9.4559451091958832E-2</v>
       </c>
       <c r="Q161">
-        <f t="shared" si="256"/>
+        <f t="shared" si="42"/>
         <v>417</v>
       </c>
       <c r="R161">
-        <f t="shared" si="257"/>
+        <f t="shared" si="48"/>
         <v>1877</v>
       </c>
       <c r="S161" s="8">
-        <f t="shared" si="258"/>
+        <f t="shared" si="49"/>
         <v>0.18177855274629467</v>
       </c>
       <c r="T161" s="8">
-        <f t="shared" si="259"/>
+        <f t="shared" si="39"/>
         <v>0.10715072112738082</v>
       </c>
       <c r="U161">
-        <f t="shared" si="260"/>
+        <f t="shared" si="43"/>
         <v>2294</v>
       </c>
       <c r="V161">
-        <f t="shared" si="261"/>
+        <f t="shared" si="44"/>
         <v>11868</v>
       </c>
       <c r="W161" s="3">
-        <f t="shared" si="262"/>
+        <f t="shared" si="45"/>
         <v>2.3171553758004719E-2</v>
       </c>
       <c r="X161">
-        <f t="shared" si="263"/>
+        <f t="shared" si="46"/>
         <v>4</v>
       </c>
       <c r="Y161">
@@ -15311,25 +15311,25 @@
         <v>70</v>
       </c>
       <c r="AH161">
-        <f t="shared" si="264"/>
+        <f t="shared" si="50"/>
         <v>95</v>
       </c>
       <c r="AI161">
-        <f t="shared" si="265"/>
+        <f t="shared" si="51"/>
         <v>27</v>
       </c>
       <c r="AJ161">
-        <f t="shared" si="266"/>
+        <f t="shared" si="52"/>
         <v>626</v>
       </c>
       <c r="AK161">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44068</v>
       </c>
       <c r="B162">
@@ -15363,43 +15363,43 @@
         <v>4</v>
       </c>
       <c r="M162" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>544392</v>
       </c>
       <c r="N162" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>9.4853859314546235E-2</v>
       </c>
       <c r="Q162">
-        <f t="shared" si="256"/>
+        <f t="shared" si="42"/>
         <v>545</v>
       </c>
       <c r="R162">
-        <f t="shared" si="257"/>
+        <f t="shared" si="48"/>
         <v>3346</v>
       </c>
       <c r="S162" s="8">
-        <f t="shared" si="258"/>
+        <f t="shared" si="49"/>
         <v>0.14006682086867128</v>
       </c>
       <c r="T162" s="8">
-        <f t="shared" si="259"/>
+        <f t="shared" si="39"/>
         <v>0.11165468403697497</v>
       </c>
       <c r="U162">
-        <f t="shared" si="260"/>
+        <f t="shared" si="43"/>
         <v>3891</v>
       </c>
       <c r="V162">
-        <f t="shared" si="261"/>
+        <f t="shared" si="44"/>
         <v>11701</v>
       </c>
       <c r="W162" s="3">
-        <f t="shared" si="262"/>
+        <f t="shared" si="45"/>
         <v>2.5211520382873259E-2</v>
       </c>
       <c r="X162">
-        <f t="shared" si="263"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="Y162">
@@ -15430,25 +15430,25 @@
         <v>70</v>
       </c>
       <c r="AH162">
-        <f t="shared" si="264"/>
+        <f t="shared" si="50"/>
         <v>95</v>
       </c>
       <c r="AI162">
-        <f t="shared" si="265"/>
+        <f t="shared" si="51"/>
         <v>27</v>
       </c>
       <c r="AJ162">
-        <f t="shared" si="266"/>
+        <f t="shared" si="52"/>
         <v>626</v>
       </c>
       <c r="AK162">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44069</v>
       </c>
       <c r="B163">
@@ -15482,43 +15482,43 @@
         <v>9</v>
       </c>
       <c r="M163" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>549681</v>
       </c>
       <c r="N163" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>9.5218499857619959E-2</v>
       </c>
       <c r="Q163">
-        <f t="shared" si="256"/>
+        <f t="shared" si="42"/>
         <v>799</v>
       </c>
       <c r="R163">
-        <f t="shared" si="257"/>
+        <f t="shared" si="48"/>
         <v>5289</v>
       </c>
       <c r="S163" s="8">
-        <f t="shared" si="258"/>
+        <f t="shared" si="49"/>
         <v>0.13124178712220763</v>
       </c>
       <c r="T163" s="8">
-        <f t="shared" si="259"/>
+        <f t="shared" si="39"/>
         <v>0.11618931005110733</v>
       </c>
       <c r="U163">
-        <f t="shared" si="260"/>
+        <f t="shared" si="43"/>
         <v>6088</v>
       </c>
       <c r="V163">
-        <f t="shared" si="261"/>
+        <f t="shared" si="44"/>
         <v>11935</v>
       </c>
       <c r="W163" s="3">
-        <f t="shared" si="262"/>
+        <f t="shared" si="45"/>
         <v>2.6225387515710095E-2</v>
       </c>
       <c r="X163">
-        <f t="shared" si="263"/>
+        <f t="shared" si="46"/>
         <v>13</v>
       </c>
       <c r="Y163">
@@ -15549,19 +15549,19 @@
         <v>72</v>
       </c>
       <c r="AH163">
-        <f t="shared" si="264"/>
+        <f t="shared" si="50"/>
         <v>91</v>
       </c>
       <c r="AI163">
-        <f t="shared" si="265"/>
+        <f t="shared" si="51"/>
         <v>31</v>
       </c>
       <c r="AJ163">
-        <f t="shared" si="266"/>
+        <f t="shared" si="52"/>
         <v>603</v>
       </c>
       <c r="AK163">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="AL163">
@@ -15576,7 +15576,7 @@
     </row>
     <row r="164" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44070</v>
       </c>
       <c r="B164">
@@ -15610,43 +15610,43 @@
         <v>6</v>
       </c>
       <c r="M164" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>555411</v>
       </c>
       <c r="N164" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>9.6175501861639812E-2</v>
       </c>
       <c r="Q164">
-        <f t="shared" ref="Q164" si="267">C164-C163</f>
+        <f t="shared" si="42"/>
         <v>1253</v>
       </c>
       <c r="R164">
-        <f t="shared" ref="R164" si="268">M164-M163</f>
+        <f t="shared" si="48"/>
         <v>5730</v>
       </c>
       <c r="S164" s="8">
-        <f t="shared" ref="S164" si="269">Q164/U164</f>
+        <f t="shared" si="49"/>
         <v>0.17943577259057711</v>
       </c>
       <c r="T164" s="8">
-        <f t="shared" ref="T164" si="270">SUM(Q158:Q164)/SUM(U158:U164)</f>
+        <f t="shared" si="39"/>
         <v>0.13981235709968201</v>
       </c>
       <c r="U164">
-        <f t="shared" ref="U164" si="271">B164-B163</f>
+        <f t="shared" si="43"/>
         <v>6983</v>
       </c>
       <c r="V164">
-        <f t="shared" ref="V164" si="272">C164-D164-E164</f>
+        <f t="shared" si="44"/>
         <v>12669</v>
       </c>
       <c r="W164" s="3">
-        <f t="shared" ref="W164" si="273">F164/V164</f>
+        <f t="shared" si="45"/>
         <v>2.4074512589786091E-2</v>
       </c>
       <c r="X164">
-        <f t="shared" ref="X164" si="274">E164-E163</f>
+        <f t="shared" si="46"/>
         <v>17</v>
       </c>
       <c r="Y164">
@@ -15677,19 +15677,19 @@
         <v>72</v>
       </c>
       <c r="AH164">
-        <f t="shared" si="264"/>
+        <f t="shared" si="50"/>
         <v>93</v>
       </c>
       <c r="AI164">
-        <f t="shared" si="265"/>
+        <f t="shared" si="51"/>
         <v>30</v>
       </c>
       <c r="AJ164">
-        <f t="shared" si="266"/>
+        <f t="shared" si="52"/>
         <v>621</v>
       </c>
       <c r="AK164">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="AL164">
@@ -15704,7 +15704,7 @@
     </row>
     <row r="165" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44071</v>
       </c>
       <c r="B165">
@@ -15738,43 +15738,43 @@
         <v>9</v>
       </c>
       <c r="M165" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>555718</v>
       </c>
       <c r="N165" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>9.9887104846716895E-2</v>
       </c>
       <c r="Q165">
-        <f t="shared" ref="Q165" si="275">C165-C164</f>
+        <f t="shared" si="42"/>
         <v>2568</v>
       </c>
       <c r="R165">
-        <f t="shared" ref="R165" si="276">M165-M164</f>
+        <f t="shared" si="48"/>
         <v>307</v>
       </c>
       <c r="S165" s="8">
-        <f t="shared" ref="S165" si="277">Q165/U165</f>
+        <f t="shared" si="49"/>
         <v>0.89321739130434785</v>
       </c>
       <c r="T165" s="8">
-        <f t="shared" ref="T165" si="278">SUM(Q159:Q165)/SUM(U159:U165)</f>
+        <f t="shared" si="39"/>
         <v>0.22004514389616903</v>
       </c>
       <c r="U165">
-        <f t="shared" ref="U165" si="279">B165-B164</f>
+        <f t="shared" si="43"/>
         <v>2875</v>
       </c>
       <c r="V165">
-        <f t="shared" ref="V165" si="280">C165-D165-E165</f>
+        <f t="shared" si="44"/>
         <v>14692</v>
       </c>
       <c r="W165" s="3">
-        <f t="shared" ref="W165" si="281">F165/V165</f>
+        <f t="shared" si="45"/>
         <v>2.0351211543697251E-2</v>
       </c>
       <c r="X165">
-        <f t="shared" ref="X165" si="282">E165-E164</f>
+        <f t="shared" si="46"/>
         <v>14</v>
       </c>
       <c r="Y165">
@@ -15805,19 +15805,19 @@
         <v>73</v>
       </c>
       <c r="AH165">
-        <f t="shared" ref="AH165" si="283">Y165-AB165-AE165</f>
+        <f t="shared" si="50"/>
         <v>98</v>
       </c>
       <c r="AI165">
-        <f t="shared" ref="AI165" si="284">Z165-AC165-AF165</f>
+        <f t="shared" si="51"/>
         <v>37</v>
       </c>
       <c r="AJ165">
-        <f t="shared" ref="AJ165" si="285">AA165-AD165-AG165</f>
+        <f t="shared" si="52"/>
         <v>652</v>
       </c>
       <c r="AK165">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="AL165">
@@ -15832,7 +15832,7 @@
     </row>
     <row r="166" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44072</v>
       </c>
       <c r="B166">
@@ -15866,43 +15866,43 @@
         <v>10</v>
       </c>
       <c r="M166" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>561637</v>
       </c>
       <c r="N166" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10099962384050838</v>
       </c>
       <c r="Q166">
-        <f t="shared" ref="Q166" si="286">C166-C165</f>
+        <f t="shared" si="42"/>
         <v>1429</v>
       </c>
       <c r="R166">
-        <f t="shared" ref="R166" si="287">M166-M165</f>
+        <f t="shared" si="48"/>
         <v>5919</v>
       </c>
       <c r="S166" s="8">
-        <f t="shared" ref="S166" si="288">Q166/U166</f>
+        <f t="shared" si="49"/>
         <v>0.19447468698965706</v>
       </c>
       <c r="T166" s="8">
-        <f t="shared" ref="T166" si="289">SUM(Q160:Q166)/SUM(U160:U166)</f>
+        <f t="shared" si="39"/>
         <v>0.22543146907063638</v>
       </c>
       <c r="U166">
-        <f t="shared" ref="U166" si="290">B166-B165</f>
+        <f t="shared" si="43"/>
         <v>7348</v>
       </c>
       <c r="V166">
-        <f t="shared" ref="V166" si="291">C166-D166-E166</f>
+        <f t="shared" si="44"/>
         <v>15596</v>
       </c>
       <c r="W166" s="3">
-        <f t="shared" ref="W166" si="292">F166/V166</f>
+        <f t="shared" si="45"/>
         <v>2.0197486535008975E-2</v>
       </c>
       <c r="X166">
-        <f t="shared" ref="X166" si="293">E166-E165</f>
+        <f t="shared" si="46"/>
         <v>17</v>
       </c>
       <c r="Y166">
@@ -15933,19 +15933,19 @@
         <v>74</v>
       </c>
       <c r="AH166">
-        <f t="shared" ref="AH166" si="294">Y166-AB166-AE166</f>
+        <f t="shared" si="50"/>
         <v>96</v>
       </c>
       <c r="AI166">
-        <f t="shared" ref="AI166" si="295">Z166-AC166-AF166</f>
+        <f t="shared" si="51"/>
         <v>42</v>
       </c>
       <c r="AJ166">
-        <f t="shared" ref="AJ166" si="296">AA166-AD166-AG166</f>
+        <f t="shared" si="52"/>
         <v>698</v>
       </c>
       <c r="AK166">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="AL166">
@@ -15960,7 +15960,7 @@
     </row>
     <row r="167" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44073</v>
       </c>
       <c r="B167">
@@ -15994,43 +15994,43 @@
         <v>12</v>
       </c>
       <c r="M167" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>566342</v>
       </c>
       <c r="N167" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10168039768671702</v>
       </c>
       <c r="Q167">
-        <f t="shared" ref="Q167:Q168" si="297">C167-C166</f>
+        <f t="shared" si="42"/>
         <v>1006</v>
       </c>
       <c r="R167">
-        <f t="shared" ref="R167:R168" si="298">M167-M166</f>
+        <f t="shared" si="48"/>
         <v>4705</v>
       </c>
       <c r="S167" s="8">
-        <f t="shared" ref="S167:S168" si="299">Q167/U167</f>
+        <f t="shared" si="49"/>
         <v>0.17615128699001925</v>
       </c>
       <c r="T167" s="8">
-        <f t="shared" ref="T167:T168" si="300">SUM(Q161:Q167)/SUM(U161:U167)</f>
+        <f t="shared" si="39"/>
         <v>0.22782040352372834</v>
       </c>
       <c r="U167">
-        <f t="shared" ref="U167:U168" si="301">B167-B166</f>
+        <f t="shared" si="43"/>
         <v>5711</v>
       </c>
       <c r="V167">
-        <f t="shared" ref="V167:V168" si="302">C167-D167-E167</f>
+        <f t="shared" si="44"/>
         <v>16468</v>
       </c>
       <c r="W167" s="3">
-        <f t="shared" ref="W167:W168" si="303">F167/V167</f>
+        <f t="shared" si="45"/>
         <v>1.9128005829487493E-2</v>
       </c>
       <c r="X167">
-        <f t="shared" ref="X167:X168" si="304">E167-E166</f>
+        <f t="shared" si="46"/>
         <v>2</v>
       </c>
       <c r="Y167">
@@ -16061,25 +16061,25 @@
         <v>74</v>
       </c>
       <c r="AH167">
-        <f t="shared" ref="AH167" si="305">Y167-AB167-AE167</f>
+        <f t="shared" si="50"/>
         <v>101</v>
       </c>
       <c r="AI167">
-        <f t="shared" ref="AI167" si="306">Z167-AC167-AF167</f>
+        <f t="shared" si="51"/>
         <v>46</v>
       </c>
       <c r="AJ167">
-        <f t="shared" ref="AJ167" si="307">AA167-AD167-AG167</f>
+        <f t="shared" si="52"/>
         <v>748</v>
       </c>
       <c r="AK167">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44074</v>
       </c>
       <c r="B168">
@@ -16113,43 +16113,43 @@
         <v>7</v>
       </c>
       <c r="M168" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>568951</v>
       </c>
       <c r="N168" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10212510099989899</v>
       </c>
       <c r="Q168">
-        <f t="shared" si="297"/>
+        <f t="shared" si="42"/>
         <v>609</v>
       </c>
       <c r="R168">
-        <f t="shared" si="298"/>
+        <f t="shared" si="48"/>
         <v>2609</v>
       </c>
       <c r="S168" s="8">
-        <f t="shared" si="299"/>
+        <f t="shared" si="49"/>
         <v>0.18924798011187072</v>
       </c>
       <c r="T168" s="8">
-        <f t="shared" si="300"/>
+        <f t="shared" si="39"/>
         <v>0.22730796920861715</v>
       </c>
       <c r="U168">
-        <f t="shared" si="301"/>
+        <f t="shared" si="43"/>
         <v>3218</v>
       </c>
       <c r="V168">
-        <f t="shared" si="302"/>
+        <f t="shared" si="44"/>
         <v>16950</v>
       </c>
       <c r="W168" s="3">
-        <f t="shared" si="303"/>
+        <f t="shared" si="45"/>
         <v>1.7699115044247787E-2</v>
       </c>
       <c r="X168">
-        <f t="shared" si="304"/>
+        <f t="shared" si="46"/>
         <v>2</v>
       </c>
       <c r="Y168">
@@ -16180,19 +16180,19 @@
         <v>74</v>
       </c>
       <c r="AH168">
-        <f t="shared" ref="AH168:AJ168" si="308">Y168-AB168-AE168</f>
+        <f t="shared" si="50"/>
         <v>105</v>
       </c>
       <c r="AI168">
-        <f t="shared" si="308"/>
+        <f t="shared" si="51"/>
         <v>45</v>
       </c>
       <c r="AJ168">
-        <f t="shared" si="308"/>
+        <f t="shared" si="52"/>
         <v>766</v>
       </c>
       <c r="AK168">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>7</v>
       </c>
       <c r="AL168">
@@ -16207,7 +16207,7 @@
     </row>
     <row r="169" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44075</v>
       </c>
       <c r="B169">
@@ -16241,43 +16241,43 @@
         <v>10</v>
       </c>
       <c r="M169" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>571703</v>
       </c>
       <c r="N169" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10264793595981793</v>
       </c>
       <c r="Q169">
-        <f t="shared" ref="Q169" si="309">C169-C168</f>
+        <f t="shared" si="42"/>
         <v>684</v>
       </c>
       <c r="R169">
-        <f t="shared" ref="R169" si="310">M169-M168</f>
+        <f t="shared" si="48"/>
         <v>2752</v>
       </c>
       <c r="S169" s="8">
-        <f t="shared" ref="S169" si="311">Q169/U169</f>
+        <f t="shared" si="49"/>
         <v>0.19906868451688009</v>
       </c>
       <c r="T169" s="8">
-        <f t="shared" ref="T169" si="312">SUM(Q163:Q169)/SUM(U163:U169)</f>
+        <f t="shared" si="39"/>
         <v>0.23410639670209485</v>
       </c>
       <c r="U169">
-        <f t="shared" ref="U169" si="313">B169-B168</f>
+        <f t="shared" si="43"/>
         <v>3436</v>
       </c>
       <c r="V169">
-        <f t="shared" ref="V169" si="314">C169-D169-E169</f>
+        <f t="shared" si="44"/>
         <v>16904</v>
       </c>
       <c r="W169" s="3">
-        <f t="shared" ref="W169" si="315">F169/V169</f>
+        <f t="shared" si="45"/>
         <v>1.8398012304779932E-2</v>
       </c>
       <c r="X169">
-        <f t="shared" ref="X169" si="316">E169-E168</f>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
       <c r="Y169">
@@ -16308,25 +16308,25 @@
         <v>75</v>
       </c>
       <c r="AH169">
-        <f t="shared" ref="AH169" si="317">Y169-AB169-AE169</f>
+        <f t="shared" si="50"/>
         <v>133</v>
       </c>
       <c r="AI169">
-        <f t="shared" ref="AI169" si="318">Z169-AC169-AF169</f>
+        <f t="shared" si="51"/>
         <v>49</v>
       </c>
       <c r="AJ169">
-        <f t="shared" ref="AJ169" si="319">AA169-AD169-AG169</f>
+        <f t="shared" si="52"/>
         <v>751</v>
       </c>
       <c r="AK169">
-        <f t="shared" si="56"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44076</v>
       </c>
       <c r="B170">
@@ -16360,43 +16360,43 @@
         <v>15</v>
       </c>
       <c r="M170" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>575501</v>
       </c>
       <c r="N170" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10287111920335718</v>
       </c>
       <c r="Q170">
-        <f t="shared" ref="Q170" si="320">C170-C169</f>
+        <f t="shared" si="42"/>
         <v>594</v>
       </c>
       <c r="R170">
-        <f t="shared" ref="R170" si="321">M170-M169</f>
+        <f t="shared" si="48"/>
         <v>3798</v>
       </c>
       <c r="S170" s="8">
-        <f t="shared" ref="S170" si="322">Q170/U170</f>
+        <f t="shared" si="49"/>
         <v>0.13524590163934427</v>
       </c>
       <c r="T170" s="8">
-        <f t="shared" ref="T170" si="323">SUM(Q164:Q170)/SUM(U164:U170)</f>
+        <f t="shared" si="39"/>
         <v>0.23976091629125815</v>
       </c>
       <c r="U170">
-        <f t="shared" ref="U170" si="324">B170-B169</f>
+        <f t="shared" si="43"/>
         <v>4392</v>
       </c>
       <c r="V170">
-        <f t="shared" ref="V170:V171" si="325">C170-D170-E170</f>
+        <f t="shared" si="44"/>
         <v>16862</v>
       </c>
       <c r="W170" s="3">
-        <f t="shared" ref="W170:W171" si="326">F170/V170</f>
+        <f t="shared" si="45"/>
         <v>1.8384533270074725E-2</v>
       </c>
       <c r="X170">
-        <f t="shared" ref="X170" si="327">E170-E169</f>
+        <f t="shared" si="46"/>
         <v>4</v>
       </c>
       <c r="Y170">
@@ -16427,19 +16427,19 @@
         <v>76</v>
       </c>
       <c r="AH170">
-        <f t="shared" ref="AH170:AH171" si="328">Y170-AB170-AE170</f>
+        <f t="shared" si="50"/>
         <v>137</v>
       </c>
       <c r="AI170">
-        <f t="shared" ref="AI170:AI171" si="329">Z170-AC170-AF170</f>
+        <f t="shared" si="51"/>
         <v>48</v>
       </c>
       <c r="AJ170">
-        <f t="shared" ref="AJ170:AJ171" si="330">AA170-AD170-AG170</f>
+        <f t="shared" si="52"/>
         <v>744</v>
       </c>
       <c r="AK170">
-        <f t="shared" ref="AK170" si="331">-(J170-J169)+L170</f>
+        <f>-(J170-J169)+L170</f>
         <v>11</v>
       </c>
       <c r="AL170">
@@ -16454,7 +16454,7 @@
     </row>
     <row r="171" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
-        <f t="shared" si="195"/>
+        <f t="shared" si="47"/>
         <v>44077</v>
       </c>
       <c r="B171">
@@ -16488,43 +16488,43 @@
         <v>13</v>
       </c>
       <c r="M171" s="7">
-        <f t="shared" si="254"/>
+        <f t="shared" si="53"/>
         <v>580286</v>
       </c>
       <c r="N171" s="4">
-        <f t="shared" si="255"/>
+        <f t="shared" si="54"/>
         <v>0.10297973115021704</v>
       </c>
       <c r="Q171">
-        <f t="shared" ref="Q171" si="332">C171-C170</f>
+        <f t="shared" si="42"/>
         <v>627</v>
       </c>
       <c r="R171">
-        <f t="shared" ref="R171" si="333">M171-M170</f>
+        <f t="shared" si="48"/>
         <v>4785</v>
       </c>
       <c r="S171" s="8">
-        <f t="shared" ref="S171" si="334">Q171/U171</f>
+        <f t="shared" si="49"/>
         <v>0.11585365853658537</v>
       </c>
       <c r="T171" s="8">
-        <f t="shared" ref="T171" si="335">SUM(Q165:Q171)/SUM(U165:U171)</f>
+        <f t="shared" si="39"/>
         <v>0.23206347246233638</v>
       </c>
       <c r="U171">
-        <f t="shared" ref="U171" si="336">B171-B170</f>
+        <f t="shared" si="43"/>
         <v>5412</v>
       </c>
       <c r="V171">
-        <f t="shared" ref="V171" si="337">C171-D171-E171</f>
+        <f t="shared" si="44"/>
         <v>16975</v>
       </c>
       <c r="W171" s="3">
-        <f t="shared" ref="W171" si="338">F171/V171</f>
+        <f t="shared" si="45"/>
         <v>1.9027982326951399E-2</v>
       </c>
       <c r="X171">
-        <f t="shared" ref="X171" si="339">E171-E170</f>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
       <c r="Y171">
@@ -16555,16 +16555,276 @@
         <v>76</v>
       </c>
       <c r="AH171">
-        <f t="shared" si="328"/>
+        <f t="shared" si="50"/>
         <v>137</v>
       </c>
       <c r="AI171">
-        <f t="shared" si="329"/>
+        <f t="shared" si="51"/>
         <v>39</v>
       </c>
       <c r="AJ171">
-        <f t="shared" si="330"/>
+        <f t="shared" si="52"/>
         <v>738</v>
+      </c>
+      <c r="AK171">
+        <f>-(J171-J170)+L171</f>
+        <v>7</v>
+      </c>
+      <c r="AL171">
+        <v>65</v>
+      </c>
+      <c r="AM171">
+        <v>65</v>
+      </c>
+      <c r="AN171">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="172" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <f t="shared" si="47"/>
+        <v>44078</v>
+      </c>
+      <c r="B172">
+        <v>654603</v>
+      </c>
+      <c r="C172">
+        <v>67844</v>
+      </c>
+      <c r="D172">
+        <v>48994</v>
+      </c>
+      <c r="E172">
+        <v>1137</v>
+      </c>
+      <c r="F172">
+        <v>317</v>
+      </c>
+      <c r="H172">
+        <v>87</v>
+      </c>
+      <c r="I172">
+        <v>41</v>
+      </c>
+      <c r="J172">
+        <v>68</v>
+      </c>
+      <c r="K172">
+        <v>16</v>
+      </c>
+      <c r="L172">
+        <v>5</v>
+      </c>
+      <c r="M172" s="7">
+        <f>B172-C172</f>
+        <v>586759</v>
+      </c>
+      <c r="N172" s="4">
+        <f>C172/B172</f>
+        <v>0.10364144374529295</v>
+      </c>
+      <c r="Q172">
+        <f t="shared" si="42"/>
+        <v>1226</v>
+      </c>
+      <c r="R172">
+        <f t="shared" si="48"/>
+        <v>6473</v>
+      </c>
+      <c r="S172" s="8">
+        <f t="shared" si="49"/>
+        <v>0.15924145992986102</v>
+      </c>
+      <c r="T172" s="8">
+        <f t="shared" si="39"/>
+        <v>0.16592325881341358</v>
+      </c>
+      <c r="U172">
+        <f t="shared" si="43"/>
+        <v>7699</v>
+      </c>
+      <c r="V172">
+        <f t="shared" si="44"/>
+        <v>17713</v>
+      </c>
+      <c r="W172" s="3">
+        <f t="shared" si="45"/>
+        <v>1.7896460226951957E-2</v>
+      </c>
+      <c r="X172">
+        <f t="shared" si="46"/>
+        <v>3</v>
+      </c>
+      <c r="Y172">
+        <v>366</v>
+      </c>
+      <c r="Z172">
+        <v>217</v>
+      </c>
+      <c r="AA172">
+        <v>3904</v>
+      </c>
+      <c r="AB172">
+        <v>220</v>
+      </c>
+      <c r="AC172">
+        <v>178</v>
+      </c>
+      <c r="AD172">
+        <v>3048</v>
+      </c>
+      <c r="AE172">
+        <v>7</v>
+      </c>
+      <c r="AF172">
+        <v>2</v>
+      </c>
+      <c r="AG172">
+        <v>76</v>
+      </c>
+      <c r="AH172">
+        <f t="shared" si="50"/>
+        <v>139</v>
+      </c>
+      <c r="AI172">
+        <f t="shared" si="51"/>
+        <v>37</v>
+      </c>
+      <c r="AJ172">
+        <f t="shared" si="52"/>
+        <v>780</v>
+      </c>
+      <c r="AK172">
+        <f>-(J172-J171)+L172</f>
+        <v>10</v>
+      </c>
+      <c r="AL172">
+        <v>68</v>
+      </c>
+      <c r="AM172">
+        <v>68</v>
+      </c>
+      <c r="AN172">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="173" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A173" s="1">
+        <f t="shared" si="47"/>
+        <v>44079</v>
+      </c>
+      <c r="B173">
+        <v>661816</v>
+      </c>
+      <c r="C173">
+        <v>68933</v>
+      </c>
+      <c r="D173">
+        <v>49487</v>
+      </c>
+      <c r="E173">
+        <v>1158</v>
+      </c>
+      <c r="F173">
+        <v>315</v>
+      </c>
+      <c r="H173">
+        <v>94</v>
+      </c>
+      <c r="I173">
+        <v>36</v>
+      </c>
+      <c r="J173">
+        <v>68</v>
+      </c>
+      <c r="K173">
+        <v>19</v>
+      </c>
+      <c r="L173">
+        <v>10</v>
+      </c>
+      <c r="M173" s="7">
+        <f>B173-C173</f>
+        <v>592883</v>
+      </c>
+      <c r="N173" s="4">
+        <f>C173/B173</f>
+        <v>0.10415734887038089</v>
+      </c>
+      <c r="Q173">
+        <f t="shared" ref="Q173" si="55">C173-C172</f>
+        <v>1089</v>
+      </c>
+      <c r="R173">
+        <f t="shared" ref="R173" si="56">M173-M172</f>
+        <v>6124</v>
+      </c>
+      <c r="S173" s="8">
+        <f t="shared" ref="S173" si="57">Q173/U173</f>
+        <v>0.15097740191321227</v>
+      </c>
+      <c r="T173" s="8">
+        <f t="shared" ref="T173" si="58">SUM(Q167:Q173)/SUM(U167:U173)</f>
+        <v>0.15735821579784795</v>
+      </c>
+      <c r="U173">
+        <f t="shared" ref="U173" si="59">B173-B172</f>
+        <v>7213</v>
+      </c>
+      <c r="V173">
+        <f t="shared" ref="V173" si="60">C173-D173-E173</f>
+        <v>18288</v>
+      </c>
+      <c r="W173" s="3">
+        <f t="shared" ref="W173" si="61">F173/V173</f>
+        <v>1.7224409448818898E-2</v>
+      </c>
+      <c r="X173">
+        <f t="shared" si="46"/>
+        <v>21</v>
+      </c>
+      <c r="Y173">
+        <v>372</v>
+      </c>
+      <c r="Z173">
+        <v>219</v>
+      </c>
+      <c r="AA173">
+        <v>3966</v>
+      </c>
+      <c r="AB173">
+        <v>222</v>
+      </c>
+      <c r="AC173">
+        <v>183</v>
+      </c>
+      <c r="AD173">
+        <v>3070</v>
+      </c>
+      <c r="AE173">
+        <v>7</v>
+      </c>
+      <c r="AF173">
+        <v>2</v>
+      </c>
+      <c r="AG173">
+        <v>78</v>
+      </c>
+      <c r="AH173">
+        <f t="shared" si="50"/>
+        <v>143</v>
+      </c>
+      <c r="AI173">
+        <f t="shared" si="51"/>
+        <v>34</v>
+      </c>
+      <c r="AJ173">
+        <f t="shared" si="52"/>
+        <v>818</v>
+      </c>
+      <c r="AK173">
+        <f>-(J173-J172)+L173</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>